<commit_message>
May 13 Commit: - Updating figures - Adding Duration workspaces and figures
</commit_message>
<xml_diff>
--- a/datasets/forest_plot_stock_apr20.xlsx
+++ b/datasets/forest_plot_stock_apr20.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Google Drive\AGGP2\Meta-analysis\aggp2_meta-analysis\meta-analysis_git\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4BC24EF2-65B5-4C4F-9B36-90F2638DD621}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FB59ED-8CF5-4203-B57C-F8200DE078A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="255" windowWidth="24825" windowHeight="15000"/>
+    <workbookView xWindow="9270" yWindow="2820" windowWidth="24825" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="forest_plot_stock_apr20" sheetId="1" r:id="rId1"/>
+    <sheet name="duration" sheetId="2" r:id="rId2"/>
+    <sheet name="depth duration" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -64,9 +74,6 @@
     <t>0 - 10 cm</t>
   </si>
   <si>
-    <t>orange</t>
-  </si>
-  <si>
     <t>Semi-Arid</t>
   </si>
   <si>
@@ -82,9 +89,6 @@
     <t>Drippers</t>
   </si>
   <si>
-    <t>cadetblue</t>
-  </si>
-  <si>
     <t>Sprinkler</t>
   </si>
   <si>
@@ -95,9 +99,6 @@
   </si>
   <si>
     <t>Coarse</t>
-  </si>
-  <si>
-    <t>#bf63bf</t>
   </si>
   <si>
     <t>Medium</t>
@@ -120,12 +121,39 @@
   <si>
     <t>30+ cm</t>
   </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>cadetblue</t>
+  </si>
+  <si>
+    <t>#bf63bf</t>
+  </si>
+  <si>
+    <t>study_druation</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>study_duration</t>
+  </si>
+  <si>
+    <t>Duration Mean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +284,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -959,11 +993,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,8 +1068,8 @@
         <f>F2+(1.96*G2)</f>
         <v>34.157911040000002</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
+      <c r="J2" t="s">
+        <v>30</v>
       </c>
       <c r="K2" s="1">
         <v>38</v>
@@ -1056,7 +1090,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
@@ -1075,8 +1109,8 @@
         <f t="shared" ref="I3:I45" si="2">F3+(1.96*G3)</f>
         <v>9.7262428920000001</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
+      <c r="J3" t="s">
+        <v>30</v>
       </c>
       <c r="K3" s="1">
         <v>105</v>
@@ -1097,7 +1131,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -1116,8 +1150,8 @@
         <f t="shared" si="2"/>
         <v>8.1960992489999995</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>14</v>
+      <c r="J4" t="s">
+        <v>30</v>
       </c>
       <c r="K4" s="1">
         <v>27</v>
@@ -1138,7 +1172,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>13</v>
@@ -1157,8 +1191,8 @@
         <f t="shared" si="2"/>
         <v>-15.547085074000002</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>14</v>
+      <c r="J5" t="s">
+        <v>30</v>
       </c>
       <c r="K5" s="1">
         <v>9</v>
@@ -1176,10 +1210,10 @@
         <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -1198,8 +1232,8 @@
         <f t="shared" si="2"/>
         <v>9.720654519</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>20</v>
+      <c r="J6" t="s">
+        <v>31</v>
       </c>
       <c r="K6" s="1">
         <v>25</v>
@@ -1217,10 +1251,10 @@
         <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
@@ -1239,8 +1273,8 @@
         <f t="shared" si="2"/>
         <v>9.7768599599999995</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>20</v>
+      <c r="J7" t="s">
+        <v>31</v>
       </c>
       <c r="K7" s="1">
         <v>81</v>
@@ -1258,10 +1292,10 @@
         <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
@@ -1280,8 +1314,8 @@
         <f t="shared" si="2"/>
         <v>18.37718851</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>20</v>
+      <c r="J8" t="s">
+        <v>31</v>
       </c>
       <c r="K8" s="1">
         <v>65</v>
@@ -1299,10 +1333,10 @@
         <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>13</v>
@@ -1321,8 +1355,8 @@
         <f t="shared" si="2"/>
         <v>13.732381986999998</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>25</v>
+      <c r="J9" t="s">
+        <v>32</v>
       </c>
       <c r="K9" s="1">
         <v>43</v>
@@ -1340,10 +1374,10 @@
         <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>13</v>
@@ -1362,8 +1396,8 @@
         <f t="shared" si="2"/>
         <v>19.296009519999998</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>25</v>
+      <c r="J10" t="s">
+        <v>32</v>
       </c>
       <c r="K10" s="1">
         <v>41</v>
@@ -1381,10 +1415,10 @@
         <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>13</v>
@@ -1404,8 +1438,8 @@
         <f t="shared" si="2"/>
         <v>10.833548903796709</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>25</v>
+      <c r="J11" t="s">
+        <v>32</v>
       </c>
       <c r="K11" s="1">
         <v>90</v>
@@ -1423,7 +1457,7 @@
         <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -1444,7 +1478,7 @@
         <v>11.309552669317885</v>
       </c>
       <c r="J12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K12">
         <v>179</v>
@@ -1468,7 +1502,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1">
         <v>46.629719999999999</v>
@@ -1484,8 +1518,8 @@
         <f t="shared" si="2"/>
         <v>70.145290399999993</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>14</v>
+      <c r="J13" t="s">
+        <v>30</v>
       </c>
       <c r="K13" s="1">
         <v>6</v>
@@ -1506,10 +1540,10 @@
         <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1">
         <v>2.9657909999999998</v>
@@ -1525,8 +1559,8 @@
         <f t="shared" si="2"/>
         <v>7.4747082799999998</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>14</v>
+      <c r="J14" t="s">
+        <v>30</v>
       </c>
       <c r="K14" s="1">
         <v>38</v>
@@ -1547,13 +1581,13 @@
         <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" t="s">
         <v>30</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1568,10 +1602,10 @@
         <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F16" s="1">
         <v>-6.2953995159999998</v>
@@ -1587,8 +1621,8 @@
         <f t="shared" si="2"/>
         <v>-6.2953995159999998</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>14</v>
+      <c r="J16" t="s">
+        <v>30</v>
       </c>
       <c r="K16" s="1">
         <v>4</v>
@@ -1606,13 +1640,13 @@
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F17" s="1">
         <v>-5.8530102499999996</v>
@@ -1628,8 +1662,8 @@
         <f t="shared" si="2"/>
         <v>-5.4745842299999996</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>20</v>
+      <c r="J17" t="s">
+        <v>31</v>
       </c>
       <c r="K17" s="1">
         <v>7</v>
@@ -1647,13 +1681,13 @@
         <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F18" s="1">
         <v>11.30980443</v>
@@ -1669,8 +1703,8 @@
         <f t="shared" si="2"/>
         <v>27.071346310000003</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>20</v>
+      <c r="J18" t="s">
+        <v>31</v>
       </c>
       <c r="K18" s="1">
         <v>16</v>
@@ -1688,13 +1722,13 @@
         <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F19" s="1">
         <v>10.075089999999999</v>
@@ -1710,8 +1744,8 @@
         <f t="shared" si="2"/>
         <v>16.47306704</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>20</v>
+      <c r="J19" t="s">
+        <v>31</v>
       </c>
       <c r="K19" s="1">
         <v>18</v>
@@ -1729,13 +1763,13 @@
         <v>37</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F20" s="1">
         <v>22.563839130000002</v>
@@ -1751,8 +1785,8 @@
         <f t="shared" si="2"/>
         <v>44.682086330000004</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>25</v>
+      <c r="J20" t="s">
+        <v>32</v>
       </c>
       <c r="K20" s="1">
         <v>10</v>
@@ -1770,13 +1804,13 @@
         <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F21" s="1">
         <v>9.0451859999999993</v>
@@ -1792,8 +1826,8 @@
         <f t="shared" si="2"/>
         <v>19.038443132879998</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>25</v>
+      <c r="J21" t="s">
+        <v>32</v>
       </c>
       <c r="K21" s="1">
         <v>17</v>
@@ -1811,13 +1845,13 @@
         <v>35</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="F22" s="1">
         <v>-0.57665650000000002</v>
@@ -1834,8 +1868,8 @@
         <f t="shared" si="2"/>
         <v>4.5675902226342604</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>25</v>
+      <c r="J22" t="s">
+        <v>32</v>
       </c>
       <c r="K22" s="1">
         <v>21</v>
@@ -1853,10 +1887,10 @@
         <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F23">
         <v>7.6520159999999997</v>
@@ -1874,7 +1908,7 @@
         <v>13.918584193363102</v>
       </c>
       <c r="J23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K23">
         <v>48</v>
@@ -1898,7 +1932,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F24" s="1">
         <v>10.60281</v>
@@ -1914,8 +1948,8 @@
         <f t="shared" si="2"/>
         <v>19.980357479999999</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>14</v>
+      <c r="J24" t="s">
+        <v>30</v>
       </c>
       <c r="K24" s="1">
         <v>27</v>
@@ -1936,10 +1970,10 @@
         <v>11</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F25" s="1">
         <v>4.4622055400000002</v>
@@ -1955,8 +1989,8 @@
         <f t="shared" si="2"/>
         <v>10.403541780000001</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>14</v>
+      <c r="J25" t="s">
+        <v>30</v>
       </c>
       <c r="K25" s="1">
         <v>44</v>
@@ -1977,10 +2011,10 @@
         <v>11</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F26" s="1">
         <v>-3.420086687</v>
@@ -1996,8 +2030,8 @@
         <f t="shared" si="2"/>
         <v>4.5251163129999998</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>14</v>
+      <c r="J26" t="s">
+        <v>30</v>
       </c>
       <c r="K26" s="1">
         <v>9</v>
@@ -2018,10 +2052,10 @@
         <v>11</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F27" s="1">
         <v>-30.299372200000001</v>
@@ -2037,8 +2071,8 @@
         <f t="shared" si="2"/>
         <v>-30.299372200000001</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>14</v>
+      <c r="J27" t="s">
+        <v>30</v>
       </c>
       <c r="K27" s="1">
         <v>4</v>
@@ -2056,13 +2090,13 @@
         <v>19</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F28" s="1">
         <v>-18.683161389999999</v>
@@ -2078,8 +2112,8 @@
         <f t="shared" si="2"/>
         <v>-13.032918469999998</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>20</v>
+      <c r="J28" t="s">
+        <v>31</v>
       </c>
       <c r="K28" s="1">
         <v>16</v>
@@ -2097,13 +2131,13 @@
         <v>18</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F29" s="1">
         <v>4.2900060550000001</v>
@@ -2119,8 +2153,8 @@
         <f t="shared" si="2"/>
         <v>11.531073175</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>20</v>
+      <c r="J29" t="s">
+        <v>31</v>
       </c>
       <c r="K29" s="1">
         <v>36</v>
@@ -2138,13 +2172,13 @@
         <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F30" s="1">
         <v>12.46271975</v>
@@ -2160,8 +2194,8 @@
         <f t="shared" si="2"/>
         <v>18.737401030000001</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>20</v>
+      <c r="J30" t="s">
+        <v>31</v>
       </c>
       <c r="K30" s="1">
         <v>29</v>
@@ -2179,13 +2213,13 @@
         <v>23</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F31" s="1">
         <v>-1.5799650000000001</v>
@@ -2201,8 +2235,8 @@
         <f t="shared" si="2"/>
         <v>15.510984120000002</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>25</v>
+      <c r="J31" t="s">
+        <v>32</v>
       </c>
       <c r="K31" s="1">
         <v>17</v>
@@ -2220,13 +2254,13 @@
         <v>22</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F32" s="1">
         <v>-0.11102049999999999</v>
@@ -2242,8 +2276,8 @@
         <f t="shared" si="2"/>
         <v>2.5243900414000002</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>25</v>
+      <c r="J32" t="s">
+        <v>32</v>
       </c>
       <c r="K32" s="1">
         <v>16</v>
@@ -2261,13 +2295,13 @@
         <v>21</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F33" s="1">
         <v>6.7522147239999999</v>
@@ -2283,8 +2317,8 @@
         <f t="shared" si="2"/>
         <v>11.243213684000001</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>25</v>
+      <c r="J33" t="s">
+        <v>32</v>
       </c>
       <c r="K33" s="1">
         <v>50</v>
@@ -2302,10 +2336,10 @@
         <v>15</v>
       </c>
       <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" t="s">
         <v>28</v>
-      </c>
-      <c r="E34" t="s">
-        <v>31</v>
       </c>
       <c r="F34">
         <v>3.9361269999999999</v>
@@ -2322,7 +2356,7 @@
         <v>8.7291535123999999</v>
       </c>
       <c r="J34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K34">
         <v>84</v>
@@ -2346,7 +2380,7 @@
         <v>12</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F35" s="1">
         <v>30.99399</v>
@@ -2362,8 +2396,8 @@
         <f t="shared" si="2"/>
         <v>46.296235279999998</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>14</v>
+      <c r="J35" t="s">
+        <v>30</v>
       </c>
       <c r="K35" s="1">
         <v>14</v>
@@ -2384,10 +2418,10 @@
         <v>11</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F36" s="1">
         <v>-0.96036207799999995</v>
@@ -2403,8 +2437,8 @@
         <f t="shared" si="2"/>
         <v>6.174300562</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>14</v>
+      <c r="J36" t="s">
+        <v>30</v>
       </c>
       <c r="K36" s="1">
         <v>24</v>
@@ -2425,10 +2459,10 @@
         <v>11</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F37" s="1">
         <v>-0.45414129600000003</v>
@@ -2444,8 +2478,8 @@
         <f t="shared" si="2"/>
         <v>0.55926768800000004</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>14</v>
+      <c r="J37" t="s">
+        <v>30</v>
       </c>
       <c r="K37" s="1">
         <v>9</v>
@@ -2466,10 +2500,10 @@
         <v>11</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F38" s="1">
         <v>-32.880313030000003</v>
@@ -2485,8 +2519,8 @@
         <f t="shared" si="2"/>
         <v>-32.880313030000003</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>14</v>
+      <c r="J38" t="s">
+        <v>30</v>
       </c>
       <c r="K38" s="1">
         <v>4</v>
@@ -2504,13 +2538,13 @@
         <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E39" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F39" s="1">
         <v>-14.520641619999999</v>
@@ -2526,8 +2560,8 @@
         <f t="shared" si="2"/>
         <v>-6.4308298199999996</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>20</v>
+      <c r="J39" t="s">
+        <v>31</v>
       </c>
       <c r="K39" s="1">
         <v>12</v>
@@ -2545,13 +2579,13 @@
         <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F40" s="1">
         <v>10.084091109999999</v>
@@ -2567,8 +2601,8 @@
         <f t="shared" si="2"/>
         <v>20.667320829999998</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>20</v>
+      <c r="J40" t="s">
+        <v>31</v>
       </c>
       <c r="K40" s="1">
         <v>24</v>
@@ -2586,13 +2620,13 @@
         <v>3</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F41" s="1">
         <v>7.7714447030000002</v>
@@ -2608,8 +2642,8 @@
         <f>F41+(1.96*G41)</f>
         <v>22.477060102999999</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>20</v>
+      <c r="J41" t="s">
+        <v>31</v>
       </c>
       <c r="K41" s="1">
         <v>12</v>
@@ -2627,13 +2661,13 @@
         <v>9</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F42" s="1">
         <v>2.430184374</v>
@@ -2649,8 +2683,8 @@
         <f t="shared" si="2"/>
         <v>23.160908373999998</v>
       </c>
-      <c r="J42" s="1" t="s">
-        <v>25</v>
+      <c r="J42" t="s">
+        <v>32</v>
       </c>
       <c r="K42" s="1">
         <v>11</v>
@@ -2668,13 +2702,13 @@
         <v>8</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E43" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F43" s="1">
         <v>7.0455129999999997</v>
@@ -2690,8 +2724,8 @@
         <f t="shared" si="2"/>
         <v>16.294345319999998</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>25</v>
+      <c r="J43" t="s">
+        <v>32</v>
       </c>
       <c r="K43" s="1">
         <v>13</v>
@@ -2709,13 +2743,13 @@
         <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F44" s="1">
         <v>-0.1658338</v>
@@ -2732,8 +2766,8 @@
         <f t="shared" si="2"/>
         <v>8.8727482663812047</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>25</v>
+      <c r="J44" t="s">
+        <v>32</v>
       </c>
       <c r="K44" s="1">
         <v>23</v>
@@ -2751,10 +2785,10 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E45" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F45">
         <v>5.397227</v>
@@ -2772,13 +2806,1632 @@
         <v>12.680195067301961</v>
       </c>
       <c r="J45" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K45">
         <v>51</v>
       </c>
       <c r="L45">
         <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0436840-D698-4036-8CA5-3443CBA61700}">
+  <dimension ref="B1:K45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6.0070670000000002</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4.70282</v>
+      </c>
+      <c r="G2" s="1">
+        <f>E2-F2</f>
+        <v>1.3042470000000002</v>
+      </c>
+      <c r="H2" s="1">
+        <f>E2+F2</f>
+        <v>10.709887</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9.8210449999999998</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.6547430000000001</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G34" si="0">E3-F3</f>
+        <v>8.1663019999999999</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H34" si="1">E3+F3</f>
+        <v>11.475788</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="1">
+        <v>122</v>
+      </c>
+      <c r="K3" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.654847</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4.7907320000000002</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.135885</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="1"/>
+        <v>6.4455790000000004</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1">
+        <v>17</v>
+      </c>
+      <c r="K4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-20.38503</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.109394</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>-22.494424000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>-18.275635999999999</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1">
+        <v>21</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-7.6327239999999996</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.2763520000000002</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.9090759999999989</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>-5.3563719999999995</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="1">
+        <v>60</v>
+      </c>
+      <c r="K6" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5.2908200000000001</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.7254879999999999</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5653320000000002</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0163080000000004</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1">
+        <v>67</v>
+      </c>
+      <c r="K7" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1">
+        <v>16.540310000000002</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3.2923119999999999</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>13.247998000000003</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>19.832622000000001</v>
+      </c>
+      <c r="I8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="1">
+        <v>32</v>
+      </c>
+      <c r="K8" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-5.227455</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2.8883169999999998</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>-8.1157719999999998</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.3391380000000002</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="1">
+        <v>49</v>
+      </c>
+      <c r="K9" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="1">
+        <v>7.0058790000000002</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.5933030000000001</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>4.4125759999999996</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>9.5991820000000008</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="1">
+        <v>45</v>
+      </c>
+      <c r="K10" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1">
+        <v>11.14789</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.8216319999999999</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>9.326258000000001</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>12.969522</v>
+      </c>
+      <c r="I11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="1">
+        <v>63</v>
+      </c>
+      <c r="K11" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12">
+        <v>5.0969189999999998</v>
+      </c>
+      <c r="F12">
+        <v>1.5187930000000001</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5781259999999997</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>6.6157120000000003</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12">
+        <v>178</v>
+      </c>
+      <c r="K12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1">
+        <v>64.558250000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3.4185490000000001</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>61.139701000000002</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>67.976799</v>
+      </c>
+      <c r="I13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="1">
+        <v>24</v>
+      </c>
+      <c r="K13" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-0.72003989999999995</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2.7611789999999998</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.4812189</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>2.0411390999999997</v>
+      </c>
+      <c r="I14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1">
+        <v>73</v>
+      </c>
+      <c r="K14" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1.373099E-3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.358525</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.3571519009999999</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.359898099</v>
+      </c>
+      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="1">
+        <v>28</v>
+      </c>
+      <c r="K15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="1">
+        <v>12.56475</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3.524435</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0403149999999997</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>16.089185000000001</v>
+      </c>
+      <c r="I18" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="1">
+        <v>78</v>
+      </c>
+      <c r="K18" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="1">
+        <v>11.21965</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5.1072230000000003</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="0"/>
+        <v>6.1124269999999994</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="1"/>
+        <v>16.326872999999999</v>
+      </c>
+      <c r="I19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="1">
+        <v>46</v>
+      </c>
+      <c r="K19" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="1">
+        <v>30.96547</v>
+      </c>
+      <c r="F20" s="1">
+        <v>7.3533499999999998</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="0"/>
+        <v>23.612120000000001</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="1"/>
+        <v>38.318820000000002</v>
+      </c>
+      <c r="I20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="1">
+        <v>27</v>
+      </c>
+      <c r="K20" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="1">
+        <v>-1.6956249999999999</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.8375060000000001</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.533131</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14188100000000015</v>
+      </c>
+      <c r="I21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="1">
+        <v>19</v>
+      </c>
+      <c r="K21" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="1">
+        <v>5.8165839999999998</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3.551412</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2651719999999997</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
+        <v>9.3679959999999998</v>
+      </c>
+      <c r="I22" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="1">
+        <v>69</v>
+      </c>
+      <c r="K22" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23">
+        <v>11.97499</v>
+      </c>
+      <c r="F23">
+        <v>2.8949220000000002</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0800680000000007</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="1"/>
+        <v>14.869911999999999</v>
+      </c>
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23">
+        <v>125</v>
+      </c>
+      <c r="K23">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="1">
+        <v>5.4327199999999998</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2.4478300000000002</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9848899999999996</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>7.8805499999999995</v>
+      </c>
+      <c r="I24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" s="1">
+        <v>42</v>
+      </c>
+      <c r="K24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="1">
+        <v>-23.630269999999999</v>
+      </c>
+      <c r="F25" s="1">
+        <v>6.3150890000000004</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>-29.945359</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
+        <v>-17.315180999999999</v>
+      </c>
+      <c r="I25" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="1">
+        <v>16</v>
+      </c>
+      <c r="K25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="1">
+        <v>-38.214350000000003</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29" s="1">
+        <v>12</v>
+      </c>
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="1">
+        <v>6.7100439999999999</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2.3167939999999998</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3932500000000001</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="1"/>
+        <v>9.0268379999999997</v>
+      </c>
+      <c r="I30" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" s="1">
+        <v>46</v>
+      </c>
+      <c r="K30" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" t="s">
+        <v>32</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="1">
+        <v>-7.561687</v>
+      </c>
+      <c r="F33" s="1">
+        <v>2.5522269999999998</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="0"/>
+        <v>-10.113913999999999</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="1"/>
+        <v>-5.0094600000000007</v>
+      </c>
+      <c r="I33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" s="1">
+        <v>50</v>
+      </c>
+      <c r="K33" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34">
+        <v>-2.584657</v>
+      </c>
+      <c r="F34">
+        <v>3.0143040000000001</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="0"/>
+        <v>-5.5989610000000001</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="1"/>
+        <v>0.42964700000000011</v>
+      </c>
+      <c r="I34" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34">
+        <v>58</v>
+      </c>
+      <c r="K34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6445275F-AC4D-48ED-8194-FAE1B6ACCDCC}">
+  <dimension ref="B1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1">
+        <v>7.3705129999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.1925439999999998</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1">
+        <v>88</v>
+      </c>
+      <c r="K2" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6.5072619999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.7242190000000002</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="1">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3.721438</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.5061089999999999</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1">
+        <v>41</v>
+      </c>
+      <c r="K4" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-2.060686</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.9022299999999999</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1">
+        <v>25</v>
+      </c>
+      <c r="K5" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6">
+        <v>5.0969189999999998</v>
+      </c>
+      <c r="F6">
+        <v>1.5187930000000001</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6">
+        <v>179</v>
+      </c>
+      <c r="K6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1">
+        <v>16.072500000000002</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4.7515830000000001</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1">
+        <v>54</v>
+      </c>
+      <c r="K7" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6.5330219999999999</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7.1072519999999999</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="1">
+        <v>19</v>
+      </c>
+      <c r="K8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6.8482950000000002</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5.5796479999999997</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="1">
+        <v>26</v>
+      </c>
+      <c r="K9" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1">
+        <v>12.568300000000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5.9170540000000003</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="1">
+        <v>26</v>
+      </c>
+      <c r="K10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11">
+        <v>11.97499</v>
+      </c>
+      <c r="F11">
+        <v>2.8949220000000002</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11">
+        <v>125</v>
+      </c>
+      <c r="K11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-6.2269709999999998</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.5142920000000002</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="1">
+        <v>37</v>
+      </c>
+      <c r="K12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1">
+        <v>20.121949999999998</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="1">
+        <v>4</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1">
+        <v>17</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16">
+        <v>-2.584657</v>
+      </c>
+      <c r="F16">
+        <v>3.0143040000000001</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16">
+        <v>58</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>